<commit_message>
Mode the default location to "Please read this first"
</commit_message>
<xml_diff>
--- a/src/files/EVA_Submission_template.V1.1.5.xlsx
+++ b/src/files/EVA_Submission_template.V1.1.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/WebstormProjects/eva-web/src/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEB10A4D-C64E-414F-995D-D491E572939E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1031688F-FFCF-694F-89D9-A54FA0F21F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17280" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -2366,18 +2366,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2387,8 +2378,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2402,9 +2405,6 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2758,8 +2758,8 @@
   </sheetPr>
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2770,8 +2770,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59"/>
-      <c r="B1" s="59"/>
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -2780,10 +2780,10 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
+      <c r="B2" s="68"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -2792,10 +2792,10 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="69" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="61"/>
+      <c r="B3" s="69"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2804,10 +2804,10 @@
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="62"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -2816,8 +2816,8 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="59"/>
-      <c r="B5" s="59"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2838,10 +2838,10 @@
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -2850,8 +2850,8 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="65"/>
-      <c r="B8" s="65"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2860,10 +2860,10 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="62"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2872,8 +2872,8 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2882,10 +2882,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="67" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="66"/>
+      <c r="B11" s="67"/>
     </row>
     <row r="12" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
@@ -2941,28 +2941,28 @@
       <c r="B18"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="63"/>
+      <c r="B19" s="62"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="62"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="63"/>
+      <c r="B21" s="62"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="63"/>
+      <c r="B22" s="62"/>
     </row>
     <row r="23" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
@@ -2971,6 +2971,11 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -2980,11 +2985,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5568,7 +5568,7 @@
   </sheetPr>
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -5820,7 +5820,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="73" t="s">
+      <c r="A33" s="61" t="s">
         <v>109</v>
       </c>
       <c r="B33" s="16" t="s">
@@ -5828,7 +5828,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="73" t="s">
+      <c r="A34" s="61" t="s">
         <v>111</v>
       </c>
       <c r="B34" s="16" t="s">
@@ -6069,12 +6069,12 @@
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" s="51"/>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="69"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="72"/>
       <c r="F1" s="38" t="s">
         <v>154</v>
       </c>
@@ -6121,64 +6121,64 @@
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" s="52"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="67" t="s">
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="70" t="s">
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70" t="s">
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="67" t="s">
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="S2" s="67"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
-      <c r="V2" s="67"/>
-      <c r="W2" s="67" t="s">
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="X2" s="67"/>
-      <c r="Y2" s="67"/>
-      <c r="Z2" s="67" t="s">
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="AA2" s="67"/>
-      <c r="AB2" s="67"/>
-      <c r="AC2" s="67"/>
-      <c r="AD2" s="67"/>
-      <c r="AE2" s="67"/>
-      <c r="AF2" s="67"/>
-      <c r="AG2" s="67"/>
-      <c r="AH2" s="67"/>
-      <c r="AI2" s="67"/>
-      <c r="AJ2" s="67" t="s">
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="70"/>
+      <c r="AF2" s="70"/>
+      <c r="AG2" s="70"/>
+      <c r="AH2" s="70"/>
+      <c r="AI2" s="70"/>
+      <c r="AJ2" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="AK2" s="67"/>
-      <c r="AL2" s="67"/>
-      <c r="AM2" s="67"/>
-      <c r="AN2" s="67"/>
-      <c r="AO2" s="67"/>
-      <c r="AP2" s="67"/>
-      <c r="AQ2" s="67"/>
-      <c r="AR2" s="67"/>
-      <c r="AS2" s="67"/>
+      <c r="AK2" s="70"/>
+      <c r="AL2" s="70"/>
+      <c r="AM2" s="70"/>
+      <c r="AN2" s="70"/>
+      <c r="AO2" s="70"/>
+      <c r="AP2" s="70"/>
+      <c r="AQ2" s="70"/>
+      <c r="AR2" s="70"/>
+      <c r="AS2" s="70"/>
     </row>
     <row r="3" spans="1:46" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
@@ -6259,10 +6259,10 @@
       <c r="Z3" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="AA3" s="71" t="s">
+      <c r="AA3" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="AB3" s="72" t="s">
+      <c r="AB3" s="60" t="s">
         <v>111</v>
       </c>
       <c r="AC3" s="46" t="s">

</xml_diff>